<commit_message>
Seperate toxic and non toxic messages
</commit_message>
<xml_diff>
--- a/prediction_2000_class.xlsx
+++ b/prediction_2000_class.xlsx
@@ -825,7 +825,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
@@ -3161,7 +3161,7 @@
         </is>
       </c>
       <c r="B171" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C171" t="inlineStr">
         <is>
@@ -3401,7 +3401,7 @@
         </is>
       </c>
       <c r="B186" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C186" t="inlineStr">
         <is>
@@ -4153,7 +4153,7 @@
         </is>
       </c>
       <c r="B233" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C233" t="inlineStr">
         <is>
@@ -4201,7 +4201,7 @@
         </is>
       </c>
       <c r="B236" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C236" t="inlineStr">
         <is>
@@ -4825,7 +4825,7 @@
         </is>
       </c>
       <c r="B275" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C275" t="inlineStr">
         <is>
@@ -5433,7 +5433,7 @@
         </is>
       </c>
       <c r="B313" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C313" t="inlineStr">
         <is>
@@ -5945,7 +5945,7 @@
         </is>
       </c>
       <c r="B345" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C345" t="inlineStr">
         <is>
@@ -6185,7 +6185,7 @@
         </is>
       </c>
       <c r="B360" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C360" t="inlineStr">
         <is>
@@ -6265,7 +6265,7 @@
         </is>
       </c>
       <c r="B365" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C365" t="inlineStr">
         <is>
@@ -6761,7 +6761,7 @@
         </is>
       </c>
       <c r="B396" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C396" t="inlineStr">
         <is>
@@ -6953,7 +6953,7 @@
         </is>
       </c>
       <c r="B408" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C408" t="inlineStr">
         <is>
@@ -7321,7 +7321,7 @@
         </is>
       </c>
       <c r="B431" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C431" t="inlineStr">
         <is>
@@ -7785,7 +7785,7 @@
         </is>
       </c>
       <c r="B460" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C460" t="inlineStr">
         <is>
@@ -8425,7 +8425,7 @@
         </is>
       </c>
       <c r="B500" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C500" t="inlineStr">
         <is>
@@ -8697,7 +8697,7 @@
         </is>
       </c>
       <c r="B517" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C517" t="inlineStr">
         <is>
@@ -9641,7 +9641,7 @@
         </is>
       </c>
       <c r="B576" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C576" t="inlineStr">
         <is>
@@ -10217,7 +10217,7 @@
         </is>
       </c>
       <c r="B612" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C612" t="inlineStr">
         <is>
@@ -13929,7 +13929,7 @@
         </is>
       </c>
       <c r="B844" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C844" t="inlineStr">
         <is>
@@ -13961,7 +13961,7 @@
         </is>
       </c>
       <c r="B846" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C846" t="inlineStr">
         <is>
@@ -14185,7 +14185,7 @@
         </is>
       </c>
       <c r="B860" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C860" t="inlineStr">
         <is>
@@ -14505,7 +14505,7 @@
         </is>
       </c>
       <c r="B880" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C880" t="inlineStr">
         <is>
@@ -15881,7 +15881,7 @@
         </is>
       </c>
       <c r="B966" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C966" t="inlineStr">
         <is>
@@ -16665,7 +16665,7 @@
         </is>
       </c>
       <c r="B1015" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1015" t="inlineStr">
         <is>
@@ -16841,7 +16841,7 @@
         </is>
       </c>
       <c r="B1026" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1026" t="inlineStr">
         <is>
@@ -16857,7 +16857,7 @@
         </is>
       </c>
       <c r="B1027" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1027" t="inlineStr">
         <is>
@@ -17209,7 +17209,7 @@
         </is>
       </c>
       <c r="B1049" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1049" t="inlineStr">
         <is>
@@ -18121,7 +18121,7 @@
         </is>
       </c>
       <c r="B1106" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1106" t="inlineStr">
         <is>
@@ -19145,7 +19145,7 @@
         </is>
       </c>
       <c r="B1170" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1170" t="inlineStr">
         <is>
@@ -19753,7 +19753,7 @@
         </is>
       </c>
       <c r="B1208" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1208" t="inlineStr">
         <is>
@@ -20105,7 +20105,7 @@
         </is>
       </c>
       <c r="B1230" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1230" t="inlineStr">
         <is>
@@ -20265,7 +20265,7 @@
         </is>
       </c>
       <c r="B1240" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1240" t="inlineStr">
         <is>
@@ -20377,7 +20377,7 @@
         </is>
       </c>
       <c r="B1247" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1247" t="inlineStr">
         <is>
@@ -22745,7 +22745,7 @@
         </is>
       </c>
       <c r="B1395" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1395" t="inlineStr">
         <is>
@@ -24105,7 +24105,7 @@
         </is>
       </c>
       <c r="B1480" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1480" t="inlineStr">
         <is>
@@ -24585,7 +24585,7 @@
         </is>
       </c>
       <c r="B1510" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1510" t="inlineStr">
         <is>
@@ -26841,7 +26841,7 @@
         </is>
       </c>
       <c r="B1651" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1651" t="inlineStr">
         <is>
@@ -27001,7 +27001,7 @@
         </is>
       </c>
       <c r="B1661" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1661" t="inlineStr">
         <is>
@@ -27305,7 +27305,7 @@
         </is>
       </c>
       <c r="B1680" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1680" t="inlineStr">
         <is>
@@ -28105,7 +28105,7 @@
         </is>
       </c>
       <c r="B1730" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1730" t="inlineStr">
         <is>
@@ -28137,7 +28137,7 @@
         </is>
       </c>
       <c r="B1732" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1732" t="inlineStr">
         <is>
@@ -28761,7 +28761,7 @@
         </is>
       </c>
       <c r="B1771" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1771" t="inlineStr">
         <is>
@@ -29065,7 +29065,7 @@
         </is>
       </c>
       <c r="B1790" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1790" t="inlineStr">
         <is>
@@ -29785,7 +29785,7 @@
         </is>
       </c>
       <c r="B1835" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1835" t="inlineStr">
         <is>
@@ -30137,7 +30137,7 @@
         </is>
       </c>
       <c r="B1857" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1857" t="inlineStr">
         <is>
@@ -30377,7 +30377,7 @@
         </is>
       </c>
       <c r="B1872" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1872" t="inlineStr">
         <is>
@@ -30857,7 +30857,7 @@
         </is>
       </c>
       <c r="B1902" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1902" t="inlineStr">
         <is>
@@ -30953,7 +30953,7 @@
         </is>
       </c>
       <c r="B1908" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1908" t="inlineStr">
         <is>

</xml_diff>